<commit_message>
Fixed bug: bad object name in restore sql could lead to uncommitted nested transaction. moved transaction sql outside of sp_executesql, from wrap into restoresubitem
</commit_message>
<xml_diff>
--- a/Med People/Restore Tree.xlsx
+++ b/Med People/Restore Tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew\Documents\SQL Server Management Studio\Restore Scripts\Med People\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DED081A-6327-4950-ABE0-1AD29EFA7F55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFA9635-789A-439C-AD75-E263A452C680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Restore Tree" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="255">
   <si>
     <t>LinkObjectToActivityHistory</t>
   </si>
@@ -511,9 +511,6 @@
     <t>04 LinkPeopleToSkills</t>
   </si>
   <si>
-    <t>05 Affiliates</t>
-  </si>
-  <si>
     <t>06 Education</t>
   </si>
   <si>
@@ -529,9 +526,6 @@
     <t>10 JobOrderClientTeams</t>
   </si>
   <si>
-    <t>11 LinkPeopleToKnownToUsers</t>
-  </si>
-  <si>
     <t>12 ProjectsCallStatus</t>
   </si>
   <si>
@@ -541,12 +535,6 @@
     <t>14 EMailAddress</t>
   </si>
   <si>
-    <t>15 ProjectsClientTeams</t>
-  </si>
-  <si>
-    <t>17 InternalInterviews</t>
-  </si>
-  <si>
     <t>18 CandidateCredentials</t>
   </si>
   <si>
@@ -559,9 +547,6 @@
     <t>21 LinkCandidatesToMPContacts</t>
   </si>
   <si>
-    <t>22 PeopleAdditionalNames</t>
-  </si>
-  <si>
     <t>23 LinkPeopleToNetWork</t>
   </si>
   <si>
@@ -577,12 +562,6 @@
     <t>27 JobOrderPresentedPeople</t>
   </si>
   <si>
-    <t>28 JobOrdersSources</t>
-  </si>
-  <si>
-    <t>29 JobOrdersTargetCompaniesCandidates</t>
-  </si>
-  <si>
     <t>30 ProjectsBenchmarkCandidates</t>
   </si>
   <si>
@@ -595,9 +574,6 @@
     <t>33 ProjectsSources</t>
   </si>
   <si>
-    <t>34 ProjectsClientEmployeesLists</t>
-  </si>
-  <si>
     <t>35 ProjectsShortLists</t>
   </si>
   <si>
@@ -607,45 +583,21 @@
     <t>37 ProjectsFileSearchCandidates</t>
   </si>
   <si>
-    <t>38 LastProjectActivity</t>
-  </si>
-  <si>
-    <t>39 ProjectTargetCompaniesCandidates</t>
-  </si>
-  <si>
     <t>40 PeopleAppliedTo</t>
   </si>
   <si>
     <t>41 LinkContactsToTask</t>
   </si>
   <si>
-    <t>42 LinkPeopleToPackage</t>
-  </si>
-  <si>
     <t>43 LinkPeopleToRates</t>
   </si>
   <si>
-    <t>44 ProjectsCandidateBlocks</t>
-  </si>
-  <si>
-    <t>45 EventSessionsInvitees</t>
-  </si>
-  <si>
-    <t>46 EventSessionVendors</t>
-  </si>
-  <si>
     <t>47 LinkCandidatesToMProjects</t>
   </si>
   <si>
     <t>48 LinkContactsToMProjects</t>
   </si>
   <si>
-    <t>49 LinkContactsToOpportunities</t>
-  </si>
-  <si>
-    <t>50 MProjectCompaniesContacts</t>
-  </si>
-  <si>
     <t>51 Addresses</t>
   </si>
   <si>
@@ -658,12 +610,6 @@
     <t>55 LinkObjectToActivityHistory</t>
   </si>
   <si>
-    <t>56 Assignments</t>
-  </si>
-  <si>
-    <t>57 Assignments</t>
-  </si>
-  <si>
     <t>58 JobOrders</t>
   </si>
   <si>
@@ -676,42 +622,6 @@
     <t>61 JobOrders</t>
   </si>
   <si>
-    <t>62 Projects</t>
-  </si>
-  <si>
-    <t>63 PositionDetails</t>
-  </si>
-  <si>
-    <t>64 LinkPositionsToRates</t>
-  </si>
-  <si>
-    <t>65 LinkJobOrderScheduleToPosition</t>
-  </si>
-  <si>
-    <t>67 Timesheets</t>
-  </si>
-  <si>
-    <t>68 PositionExpenses</t>
-  </si>
-  <si>
-    <t>69 JobOrderPositionTeams</t>
-  </si>
-  <si>
-    <t>70 Task</t>
-  </si>
-  <si>
-    <t>72 LinkInterviewersToClientInterview</t>
-  </si>
-  <si>
-    <t>76 Task</t>
-  </si>
-  <si>
-    <t>77 LinkInternalInterviewsToResults</t>
-  </si>
-  <si>
-    <t>78 LinkSkillsToInternalInterview</t>
-  </si>
-  <si>
     <t>via ProjectsInternalInterviewLists where Done = 0</t>
   </si>
   <si>
@@ -745,9 +655,6 @@
     <t>NESTED - People.HomeAddressesID, BusinessAddressesID, AlternativeAddressesID. MED CUSTOM</t>
   </si>
   <si>
-    <t>MailingAddresses, LinkAddresstoMCRContract, Positions update</t>
-  </si>
-  <si>
     <t>Interview, CandidateCredentials, CandidateReferences</t>
   </si>
   <si>
@@ -890,13 +797,19 @@
   </si>
   <si>
     <t>TaskID = TaskID</t>
+  </si>
+  <si>
+    <t>63 LinkCredentialsToJobOrders</t>
+  </si>
+  <si>
+    <t>covered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -913,6 +826,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1050,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1079,6 +1006,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1361,9 +1295,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,7 +1367,7 @@
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="30" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1449,7 +1383,7 @@
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="30" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1459,7 +1393,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="30" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1469,33 +1403,33 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="30" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="30" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>242</v>
+      <c r="F11" s="34" t="s">
+        <v>211</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="30" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1505,12 +1439,12 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="30" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="30" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="21" t="s">
@@ -1552,15 +1486,15 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F22" s="21" t="s">
-        <v>237</v>
+      <c r="F22" s="27" t="s">
+        <v>206</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="30" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="21" t="s">
@@ -1574,10 +1508,10 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="31" t="s">
         <v>128</v>
       </c>
       <c r="G24" s="5" t="s">
@@ -1592,40 +1526,43 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
-      <c r="F25" s="21" t="s">
-        <v>239</v>
+      <c r="F25" s="32" t="s">
+        <v>208</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="I25" s="18"/>
-      <c r="J25" s="21" t="s">
-        <v>237</v>
+      <c r="J25" s="32" t="s">
+        <v>206</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="29" t="s">
         <v>128</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>245</v>
+        <v>214</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
-      <c r="J27" s="21" t="s">
+      <c r="J27" s="32" t="s">
         <v>6</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="M27" s="5" t="s">
         <v>145</v>
@@ -1663,7 +1600,7 @@
         <v>127</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>6</v>
@@ -1676,7 +1613,7 @@
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="30" t="s">
         <v>54</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -1684,7 +1621,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="30" t="s">
         <v>58</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -1698,7 +1635,7 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="30" t="s">
         <v>59</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -1706,7 +1643,7 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="30" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="5" t="s">
@@ -1731,7 +1668,7 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="30" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1742,7 +1679,7 @@
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="30" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -1750,21 +1687,21 @@
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="30" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="21" t="s">
-        <v>237</v>
+      <c r="F39" s="28" t="s">
+        <v>206</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -1772,7 +1709,7 @@
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -1796,7 +1733,7 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="31" t="s">
         <v>44</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -1810,7 +1747,7 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="31" t="s">
         <v>45</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -1832,7 +1769,7 @@
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="31" t="s">
         <v>46</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -1846,7 +1783,7 @@
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="31" t="s">
         <v>47</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -1860,7 +1797,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="31" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1874,21 +1811,21 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="31" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="31" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -1902,7 +1839,7 @@
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="31" t="s">
         <v>52</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -1916,7 +1853,7 @@
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="31" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="5" t="s">
@@ -1924,7 +1861,7 @@
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="31" t="s">
         <v>51</v>
       </c>
       <c r="C54" s="5" t="s">
@@ -1938,7 +1875,7 @@
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="30" t="s">
         <v>60</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -1952,7 +1889,7 @@
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -1968,7 +1905,7 @@
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="30" t="s">
         <v>65</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -2000,7 +1937,7 @@
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="31" t="s">
         <v>16</v>
       </c>
       <c r="C62" s="5" t="s">
@@ -2008,7 +1945,7 @@
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="21" t="s">
+      <c r="B63" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C63" s="5" t="s">
@@ -2030,7 +1967,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="21" t="s">
+      <c r="B65" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2038,14 +1975,11 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="30" t="s">
         <v>29</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2067,7 +2001,7 @@
       <c r="A69" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C69" s="5" t="s">
@@ -2089,7 +2023,7 @@
       <c r="A71" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C71" s="17" t="s">
@@ -2142,7 +2076,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="30" t="s">
         <v>1</v>
       </c>
       <c r="C75" s="17" t="s">
@@ -2198,7 +2132,7 @@
       <c r="J79" s="12"/>
     </row>
     <row r="80" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="23" t="s">
+      <c r="B80" s="33" t="s">
         <v>85</v>
       </c>
       <c r="E80" s="11" t="s">
@@ -2208,7 +2142,7 @@
       <c r="J80" s="12"/>
     </row>
     <row r="81" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="23" t="s">
+      <c r="B81" s="33" t="s">
         <v>85</v>
       </c>
       <c r="E81" s="17" t="s">
@@ -2218,7 +2152,7 @@
       <c r="J81" s="12"/>
     </row>
     <row r="82" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="23" t="s">
+      <c r="B82" s="33" t="s">
         <v>85</v>
       </c>
       <c r="E82" s="17" t="s">
@@ -2228,7 +2162,7 @@
       <c r="J82" s="12"/>
     </row>
     <row r="83" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="23" t="s">
+      <c r="B83" s="33" t="s">
         <v>85</v>
       </c>
       <c r="E83" s="17" t="s">
@@ -2238,7 +2172,7 @@
       <c r="J83" s="12"/>
     </row>
     <row r="84" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="24" t="s">
+      <c r="B84" s="25" t="s">
         <v>86</v>
       </c>
       <c r="E84" s="3" t="s">
@@ -2297,7 +2231,7 @@
   <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2309,10 +2243,10 @@
   <sheetData>
     <row r="1" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F1" t="s">
-        <v>256</v>
+        <v>225</v>
       </c>
       <c r="G1" t="s">
         <v>107</v>
@@ -2322,42 +2256,42 @@
         <v>PositionDetails</v>
       </c>
       <c r="I1" t="s">
-        <v>257</v>
+        <v>226</v>
       </c>
       <c r="J1" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K1" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="L1" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M1" t="s">
         <v>83</v>
       </c>
       <c r="N1" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O1" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="P1" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q1" t="s">
         <v>31</v>
       </c>
       <c r="R1" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F2" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G2" t="s">
         <v>108</v>
@@ -2367,42 +2301,42 @@
         <v>LinkPositionsToRates</v>
       </c>
       <c r="I2" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="J2" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K2" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="L2" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M2" t="s">
         <v>83</v>
       </c>
       <c r="N2" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O2" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="P2" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q2" t="s">
         <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G3" t="s">
         <v>109</v>
@@ -2412,42 +2346,42 @@
         <v>#N/A</v>
       </c>
       <c r="I3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="J3" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K3" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="L3" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M3" t="s">
         <v>83</v>
       </c>
       <c r="N3" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O3" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="P3" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q3" t="s">
         <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F4" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G4" t="s">
         <v>110</v>
@@ -2457,42 +2391,42 @@
         <v>LinkJobOrderToWorksteps</v>
       </c>
       <c r="I4" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="J4" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K4" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="L4" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M4" t="s">
         <v>83</v>
       </c>
       <c r="N4" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O4" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="P4" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q4" t="s">
         <v>31</v>
       </c>
       <c r="R4" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F5" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G5" t="s">
         <v>111</v>
@@ -2502,42 +2436,42 @@
         <v>Timesheets</v>
       </c>
       <c r="I5" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="J5" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K5" t="s">
-        <v>265</v>
+        <v>234</v>
       </c>
       <c r="L5" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M5" t="s">
         <v>83</v>
       </c>
       <c r="N5" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O5" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="P5" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q5" t="s">
         <v>31</v>
       </c>
       <c r="R5" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G6" t="s">
         <v>112</v>
@@ -2547,42 +2481,42 @@
         <v>PositionExpenses</v>
       </c>
       <c r="I6" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="J6" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K6" t="s">
-        <v>267</v>
+        <v>236</v>
       </c>
       <c r="L6" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M6" t="s">
         <v>83</v>
       </c>
       <c r="N6" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O6" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="P6" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q6" t="s">
         <v>31</v>
       </c>
       <c r="R6" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F7" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G7" t="s">
         <v>113</v>
@@ -2592,42 +2526,42 @@
         <v>#N/A</v>
       </c>
       <c r="I7" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="J7" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K7" t="s">
-        <v>269</v>
+        <v>238</v>
       </c>
       <c r="L7" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M7" t="s">
         <v>83</v>
       </c>
       <c r="N7" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O7" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="P7" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q7" t="s">
         <v>31</v>
       </c>
       <c r="R7" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F8" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G8" t="s">
         <v>130</v>
@@ -2637,42 +2571,42 @@
         <v>LinkAddressToDistList</v>
       </c>
       <c r="I8" t="s">
-        <v>270</v>
+        <v>239</v>
       </c>
       <c r="J8" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K8" t="s">
         <v>140</v>
       </c>
       <c r="L8" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M8" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="N8" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O8" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
       <c r="P8" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q8" t="s">
         <v>31</v>
       </c>
       <c r="R8" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F9" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G9" t="s">
         <v>130</v>
@@ -2682,42 +2616,42 @@
         <v>LinkAddressToDistList</v>
       </c>
       <c r="I9" t="s">
-        <v>270</v>
+        <v>239</v>
       </c>
       <c r="J9" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K9" t="s">
         <v>140</v>
       </c>
       <c r="L9" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M9" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="N9" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O9" t="s">
-        <v>273</v>
+        <v>242</v>
       </c>
       <c r="P9" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q9" t="s">
         <v>31</v>
       </c>
       <c r="R9" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F10" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G10" t="s">
         <v>121</v>
@@ -2727,42 +2661,42 @@
         <v>EmailMsgRecipients</v>
       </c>
       <c r="I10" t="s">
-        <v>274</v>
+        <v>243</v>
       </c>
       <c r="J10" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K10" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
       <c r="L10" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M10" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="N10" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O10" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
       <c r="P10" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q10" t="s">
         <v>31</v>
       </c>
       <c r="R10" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F11" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G11" t="s">
         <v>136</v>
@@ -2772,42 +2706,42 @@
         <v>EmailMsgAttachments</v>
       </c>
       <c r="I11" t="s">
-        <v>278</v>
+        <v>247</v>
       </c>
       <c r="J11" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K11" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="L11" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M11" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="N11" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O11" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
       <c r="P11" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q11" t="s">
         <v>31</v>
       </c>
       <c r="R11" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F12" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G12" t="s">
         <v>0</v>
@@ -2817,48 +2751,48 @@
         <v>LinkObjectToActivityHistory</v>
       </c>
       <c r="I12" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="J12" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K12" t="s">
         <v>34</v>
       </c>
       <c r="L12" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M12" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="N12" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O12" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="P12" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q12" t="s">
         <v>31</v>
       </c>
       <c r="R12" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="S12" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="T12" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F13" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G13" t="s">
         <v>134</v>
@@ -2868,42 +2802,42 @@
         <v>#N/A</v>
       </c>
       <c r="I13" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="J13" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="K13" t="s">
         <v>141</v>
       </c>
       <c r="L13" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M13" t="s">
         <v>127</v>
       </c>
       <c r="N13" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="O13" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="P13" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="Q13" t="s">
         <v>31</v>
       </c>
       <c r="R13" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="F14" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G14" t="s">
         <v>135</v>
@@ -2915,7 +2849,7 @@
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
@@ -2925,27 +2859,27 @@
         <v>LinkContactsToMProjects</v>
       </c>
       <c r="F15" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="G15" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="H15" t="s">
         <v>31</v>
       </c>
       <c r="I15" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="J15" t="s">
         <v>31</v>
       </c>
       <c r="K15" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="D16" t="s">
         <v>73</v>
@@ -2955,27 +2889,27 @@
         <v>LinkContactsToOpportunities</v>
       </c>
       <c r="F16" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="G16" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="H16" t="s">
         <v>31</v>
       </c>
       <c r="I16" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="J16" t="s">
         <v>31</v>
       </c>
       <c r="K16" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -2985,27 +2919,27 @@
         <v>MProjectCompaniesContacts</v>
       </c>
       <c r="F17" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="G17" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
       </c>
       <c r="I17" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="J17" t="s">
         <v>31</v>
       </c>
       <c r="K17" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -3015,33 +2949,33 @@
         <v>#N/A</v>
       </c>
       <c r="F18" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="G18" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
       </c>
       <c r="I18" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="J18" t="s">
         <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="L18" t="s">
         <v>26</v>
       </c>
       <c r="M18" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
@@ -3051,33 +2985,33 @@
         <v>#N/A</v>
       </c>
       <c r="F19" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="G19" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
       </c>
       <c r="I19" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="J19" t="s">
         <v>34</v>
       </c>
       <c r="K19" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="L19" t="s">
         <v>26</v>
       </c>
       <c r="M19" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="D20" t="s">
         <v>2</v>
@@ -3087,33 +3021,33 @@
         <v>#N/A</v>
       </c>
       <c r="F20" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="G20" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="H20" t="s">
         <v>34</v>
       </c>
       <c r="I20" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="J20" t="s">
         <v>34</v>
       </c>
       <c r="K20" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="L20" t="s">
         <v>26</v>
       </c>
       <c r="M20" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="D21" t="s">
         <v>128</v>
@@ -3123,22 +3057,22 @@
         <v>#N/A</v>
       </c>
       <c r="F21" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="G21" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="H21" t="s">
         <v>34</v>
       </c>
       <c r="I21" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="J21" t="s">
         <v>34</v>
       </c>
       <c r="K21" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -3467,289 +3401,289 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C61" t="s">
         <v>84</v>
       </c>
       <c r="D61" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="E61" t="s">
         <v>31</v>
       </c>
       <c r="F61" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G61" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="H61" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="I61" t="s">
         <v>31</v>
       </c>
       <c r="J61" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="K61" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="L61" t="s">
         <v>31</v>
       </c>
       <c r="M61" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="N61" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C62" t="s">
         <v>84</v>
       </c>
       <c r="D62" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="E62" t="s">
         <v>72</v>
       </c>
       <c r="F62" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G62" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="H62" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="I62" t="s">
         <v>72</v>
       </c>
       <c r="J62" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="K62" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="L62" t="s">
         <v>31</v>
       </c>
       <c r="M62" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="N62" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C63" t="s">
         <v>85</v>
       </c>
       <c r="D63" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="E63" t="s">
         <v>87</v>
       </c>
       <c r="F63" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G63" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="H63" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="I63" t="s">
         <v>87</v>
       </c>
       <c r="J63" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="K63" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="L63" t="s">
         <v>31</v>
       </c>
       <c r="M63" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="N63" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C64" t="s">
         <v>85</v>
       </c>
       <c r="D64" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="E64" t="s">
         <v>88</v>
       </c>
       <c r="F64" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G64" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="H64" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="I64" t="s">
         <v>88</v>
       </c>
       <c r="J64" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="K64" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="L64" t="s">
         <v>31</v>
       </c>
       <c r="M64" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="N64" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C65" t="s">
         <v>85</v>
       </c>
       <c r="D65" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="E65" t="s">
         <v>89</v>
       </c>
       <c r="F65" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G65" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="H65" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="I65" t="s">
         <v>89</v>
       </c>
       <c r="J65" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="K65" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="L65" t="s">
         <v>31</v>
       </c>
       <c r="M65" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="N65" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C66" t="s">
         <v>85</v>
       </c>
       <c r="D66" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="E66" t="s">
         <v>90</v>
       </c>
       <c r="F66" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G66" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="H66" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="I66" t="s">
         <v>90</v>
       </c>
       <c r="J66" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="K66" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="L66" t="s">
         <v>31</v>
       </c>
       <c r="M66" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="N66" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
       </c>
       <c r="D67" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="E67" t="s">
         <v>91</v>
       </c>
       <c r="F67" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G67" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="H67" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="I67" t="s">
         <v>91</v>
       </c>
       <c r="J67" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="K67" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="L67" t="s">
         <v>31</v>
       </c>
       <c r="M67" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="N67" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3761,8 +3695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4650E00-41D3-4D18-8520-046A79031E4C}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3779,6 +3713,10 @@
       <c r="C1" t="s">
         <v>31</v>
       </c>
+      <c r="G1" t="e">
+        <f t="shared" ref="G1:G66" si="0">VLOOKUP($F$2,C1:D1,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -3788,20 +3726,16 @@
         <v>153</v>
       </c>
       <c r="C2">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D2" t="s">
         <v>153</v>
       </c>
       <c r="E2">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="F2">
-        <v>78181</v>
-      </c>
-      <c r="G2" t="e">
-        <f>VLOOKUP($F$2,C2:D2,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>26755</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3813,17 +3747,13 @@
         <v>154</v>
       </c>
       <c r="C3">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D3" t="s">
         <v>154</v>
       </c>
       <c r="E3">
-        <v>79632</v>
-      </c>
-      <c r="G3" t="e">
-        <f t="shared" ref="G3:G66" si="0">VLOOKUP($F$2,C3:D3,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>9411067</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3835,17 +3765,13 @@
         <v>155</v>
       </c>
       <c r="C4">
-        <v>95324</v>
+        <v>9411067</v>
       </c>
       <c r="D4" t="s">
         <v>155</v>
       </c>
       <c r="E4">
-        <v>52042</v>
-      </c>
-      <c r="G4" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>9402686</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3857,14 +3783,13 @@
         <v>156</v>
       </c>
       <c r="C5">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D5" t="s">
         <v>156</v>
       </c>
-      <c r="G5" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="E5">
+        <v>9407570</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3872,17 +3797,8 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6">
-        <v>95324</v>
-      </c>
-      <c r="D6" t="s">
-        <v>157</v>
-      </c>
       <c r="E6">
-        <v>78177</v>
+        <v>9411142</v>
       </c>
       <c r="G6" t="e">
         <f t="shared" si="0"/>
@@ -3895,20 +3811,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7">
-        <v>78203</v>
-      </c>
-      <c r="G7" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3917,20 +3829,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8">
-        <v>79632</v>
+        <v>9402686</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E8">
-        <v>77010</v>
-      </c>
-      <c r="G8" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3939,20 +3847,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E9">
-        <v>78846</v>
-      </c>
-      <c r="G9" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>9401060</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3961,20 +3865,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10">
-        <v>95324</v>
+        <v>9407570</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E10">
-        <v>78858</v>
-      </c>
-      <c r="G10" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3983,20 +3883,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11">
-        <v>52042</v>
+        <v>9411142</v>
       </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E11">
-        <v>78270</v>
-      </c>
-      <c r="G11" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>9410837</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4004,17 +3900,8 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12">
-        <v>79632</v>
-      </c>
-      <c r="D12" t="s">
-        <v>163</v>
-      </c>
       <c r="E12">
-        <v>66825</v>
+        <v>1222</v>
       </c>
       <c r="G12" t="e">
         <f t="shared" si="0"/>
@@ -4027,20 +3914,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C13">
-        <v>95324</v>
+        <v>9411067</v>
       </c>
       <c r="D13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E13">
-        <v>40710</v>
-      </c>
-      <c r="G13" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>9404825</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4049,20 +3932,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C14">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E14">
-        <v>78517</v>
-      </c>
-      <c r="G14" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>9410642</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4071,20 +3950,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C15">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E15">
-        <v>78181</v>
-      </c>
-      <c r="G15" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>9400917</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4092,14 +3967,8 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C16">
-        <v>95324</v>
-      </c>
-      <c r="D16" t="s">
-        <v>167</v>
+      <c r="E16">
+        <v>9406060</v>
       </c>
       <c r="G16" t="e">
         <f t="shared" si="0"/>
@@ -4111,6 +3980,9 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
+      <c r="E17">
+        <v>26755</v>
+      </c>
       <c r="G17" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4121,15 +3993,6 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18">
-        <v>78177</v>
-      </c>
-      <c r="D18" t="s">
-        <v>168</v>
-      </c>
       <c r="G18" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4141,17 +4004,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C19">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D19" t="s">
-        <v>169</v>
-      </c>
-      <c r="G19" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4160,17 +4019,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C20">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
-      </c>
-      <c r="G20" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -4179,17 +4034,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C21">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
-      </c>
-      <c r="G21" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4198,17 +4049,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C22">
-        <v>95324</v>
+        <v>2290</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
-      </c>
-      <c r="G22" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -4216,15 +4063,6 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23">
-        <v>95324</v>
-      </c>
-      <c r="D23" t="s">
-        <v>173</v>
-      </c>
       <c r="G23" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4236,17 +4074,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C24">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D24" t="s">
-        <v>174</v>
-      </c>
-      <c r="G24" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -4255,17 +4089,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C25">
-        <v>95324</v>
+        <v>9402686</v>
       </c>
       <c r="D25" t="s">
-        <v>175</v>
-      </c>
-      <c r="G25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4274,17 +4104,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C26">
-        <v>79632</v>
+        <v>9402686</v>
       </c>
       <c r="D26" t="s">
-        <v>176</v>
-      </c>
-      <c r="G26" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4293,17 +4119,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C27">
-        <v>95324</v>
+        <v>2290</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
-      </c>
-      <c r="G27" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4312,17 +4134,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C28">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
-      </c>
-      <c r="G28" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -4330,15 +4148,6 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>179</v>
-      </c>
-      <c r="C29">
-        <v>95324</v>
-      </c>
-      <c r="D29" t="s">
-        <v>179</v>
-      </c>
       <c r="G29" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4349,15 +4158,6 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>180</v>
-      </c>
-      <c r="C30">
-        <v>95324</v>
-      </c>
-      <c r="D30" t="s">
-        <v>180</v>
-      </c>
       <c r="G30" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4369,17 +4169,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C31">
-        <v>95324</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>181</v>
-      </c>
-      <c r="G31" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -4388,17 +4184,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C32">
-        <v>95324</v>
+        <v>9401060</v>
       </c>
       <c r="D32" t="s">
-        <v>182</v>
-      </c>
-      <c r="G32" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -4407,17 +4199,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C33">
-        <v>95324</v>
+        <v>9401060</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
-      </c>
-      <c r="G33" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -4426,17 +4214,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C34">
-        <v>95324</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>184</v>
-      </c>
-      <c r="G34" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -4444,19 +4228,6 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>185</v>
-      </c>
-      <c r="C35">
-        <v>95324</v>
-      </c>
-      <c r="D35" t="s">
-        <v>185</v>
-      </c>
-      <c r="G35" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -4464,17 +4235,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C36">
-        <v>95324</v>
+        <v>9401060</v>
       </c>
       <c r="D36" t="s">
-        <v>186</v>
-      </c>
-      <c r="G36" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -4483,17 +4250,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C37">
-        <v>95324</v>
+        <v>9401060</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
-      </c>
-      <c r="G37" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -4502,17 +4265,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C38">
-        <v>95324</v>
+        <v>9410837</v>
       </c>
       <c r="D38" t="s">
-        <v>188</v>
-      </c>
-      <c r="G38" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -4520,38 +4279,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>189</v>
-      </c>
-      <c r="C39">
-        <v>95324</v>
-      </c>
-      <c r="D39" t="s">
-        <v>189</v>
-      </c>
-      <c r="G39" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>190</v>
-      </c>
-      <c r="C40">
-        <v>95324</v>
-      </c>
-      <c r="D40" t="s">
-        <v>190</v>
-      </c>
-      <c r="G40" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -4559,17 +4292,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C41">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D41" t="s">
-        <v>191</v>
-      </c>
-      <c r="G41" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -4578,17 +4307,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C42">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D42" t="s">
-        <v>192</v>
-      </c>
-      <c r="G42" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -4596,15 +4321,6 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B43" t="s">
-        <v>193</v>
-      </c>
-      <c r="C43">
-        <v>78203</v>
-      </c>
-      <c r="D43" t="s">
-        <v>193</v>
-      </c>
       <c r="G43" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4616,13 +4332,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C44">
-        <v>95324</v>
+        <v>1222</v>
       </c>
       <c r="D44" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G44" t="e">
         <f t="shared" si="0"/>
@@ -4634,15 +4350,6 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>195</v>
-      </c>
-      <c r="C45">
-        <v>95324</v>
-      </c>
-      <c r="D45" t="s">
-        <v>195</v>
-      </c>
       <c r="G45" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4653,15 +4360,6 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>196</v>
-      </c>
-      <c r="C46">
-        <v>95324</v>
-      </c>
-      <c r="D46" t="s">
-        <v>196</v>
-      </c>
       <c r="G46" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4672,15 +4370,6 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B47" t="s">
-        <v>197</v>
-      </c>
-      <c r="C47">
-        <v>95324</v>
-      </c>
-      <c r="D47" t="s">
-        <v>197</v>
-      </c>
       <c r="G47" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4692,17 +4381,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="C48">
-        <v>95324</v>
+        <v>2290</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
-      </c>
-      <c r="G48" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -4711,17 +4396,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C49">
-        <v>95324</v>
+        <v>9404825</v>
       </c>
       <c r="D49" t="s">
-        <v>199</v>
-      </c>
-      <c r="G49" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -4729,15 +4410,6 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B50" t="s">
-        <v>200</v>
-      </c>
-      <c r="C50">
-        <v>95324</v>
-      </c>
-      <c r="D50" t="s">
-        <v>200</v>
-      </c>
       <c r="G50" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4748,15 +4420,6 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B51" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51">
-        <v>95324</v>
-      </c>
-      <c r="D51" t="s">
-        <v>201</v>
-      </c>
       <c r="G51" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4768,17 +4431,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C52">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D52" t="s">
-        <v>202</v>
-      </c>
-      <c r="G52" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -4787,17 +4446,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="C53">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D53" t="s">
-        <v>203</v>
-      </c>
-      <c r="G53" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -4806,17 +4461,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C54">
-        <v>95324</v>
+        <v>9402686</v>
       </c>
       <c r="D54" t="s">
-        <v>204</v>
-      </c>
-      <c r="G54" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -4835,17 +4486,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="C56">
-        <v>95324</v>
+        <v>9404017</v>
       </c>
       <c r="D56" t="s">
-        <v>205</v>
-      </c>
-      <c r="G56" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -4853,15 +4500,6 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>206</v>
-      </c>
-      <c r="C57">
-        <v>77010</v>
-      </c>
-      <c r="D57" t="s">
-        <v>206</v>
-      </c>
       <c r="G57" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4872,15 +4510,6 @@
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B58" t="s">
-        <v>207</v>
-      </c>
-      <c r="C58">
-        <v>78846</v>
-      </c>
-      <c r="D58" t="s">
-        <v>207</v>
-      </c>
       <c r="G58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4892,17 +4521,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="C59">
-        <v>79632</v>
+        <v>9410642</v>
       </c>
       <c r="D59" t="s">
-        <v>208</v>
-      </c>
-      <c r="G59" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -4911,13 +4536,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="C60">
-        <v>79632</v>
+        <v>9400917</v>
       </c>
       <c r="D60" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="G60" t="e">
         <f t="shared" si="0"/>
@@ -4930,13 +4555,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="C61">
-        <v>79632</v>
+        <v>9406060</v>
       </c>
       <c r="D61" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="G61" t="e">
         <f t="shared" si="0"/>
@@ -4949,13 +4574,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="C62">
-        <v>78177</v>
+        <v>9406060</v>
       </c>
       <c r="D62" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="G62" t="e">
         <f t="shared" si="0"/>
@@ -4967,15 +4592,6 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B63" t="s">
-        <v>212</v>
-      </c>
-      <c r="C63">
-        <v>95324</v>
-      </c>
-      <c r="D63" t="s">
-        <v>212</v>
-      </c>
       <c r="G63" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -4987,17 +4603,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>213</v>
+        <v>253</v>
       </c>
       <c r="C64">
-        <v>95324</v>
+        <v>26755</v>
       </c>
       <c r="D64" t="s">
-        <v>213</v>
-      </c>
-      <c r="G64" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>253</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -5005,15 +4617,6 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B65" t="s">
-        <v>214</v>
-      </c>
-      <c r="C65">
-        <v>95324</v>
-      </c>
-      <c r="D65" t="s">
-        <v>214</v>
-      </c>
       <c r="G65" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -5024,15 +4627,6 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="B66" t="s">
-        <v>215</v>
-      </c>
-      <c r="C66">
-        <v>78858</v>
-      </c>
-      <c r="D66" t="s">
-        <v>215</v>
-      </c>
       <c r="G66" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -5053,15 +4647,6 @@
         <f t="shared" ref="A68:A79" si="3">A67+1</f>
         <v>67</v>
       </c>
-      <c r="B68" t="s">
-        <v>216</v>
-      </c>
-      <c r="C68">
-        <v>78270</v>
-      </c>
-      <c r="D68" t="s">
-        <v>216</v>
-      </c>
       <c r="G68" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
@@ -5072,15 +4657,6 @@
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="B69" t="s">
-        <v>217</v>
-      </c>
-      <c r="C69">
-        <v>66825</v>
-      </c>
-      <c r="D69" t="s">
-        <v>217</v>
-      </c>
       <c r="G69" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
@@ -5091,15 +4667,6 @@
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="B70" t="s">
-        <v>218</v>
-      </c>
-      <c r="C70">
-        <v>40710</v>
-      </c>
-      <c r="D70" t="s">
-        <v>218</v>
-      </c>
       <c r="G70" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
@@ -5110,15 +4677,6 @@
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="B71" t="s">
-        <v>219</v>
-      </c>
-      <c r="C71">
-        <v>78270</v>
-      </c>
-      <c r="D71" t="s">
-        <v>219</v>
-      </c>
       <c r="G71" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
@@ -5139,15 +4697,6 @@
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="B73" t="s">
-        <v>220</v>
-      </c>
-      <c r="C73">
-        <v>78517</v>
-      </c>
-      <c r="D73" t="s">
-        <v>220</v>
-      </c>
       <c r="G73" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
@@ -5188,15 +4737,6 @@
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="B77" t="s">
-        <v>221</v>
-      </c>
-      <c r="C77">
-        <v>95324</v>
-      </c>
-      <c r="D77" t="s">
-        <v>221</v>
-      </c>
       <c r="G77" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
@@ -5207,15 +4747,6 @@
         <f t="shared" si="3"/>
         <v>77</v>
       </c>
-      <c r="B78" t="s">
-        <v>222</v>
-      </c>
-      <c r="C78">
-        <v>95324</v>
-      </c>
-      <c r="D78" t="s">
-        <v>222</v>
-      </c>
       <c r="G78" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
@@ -5226,18 +4757,9 @@
         <f t="shared" si="3"/>
         <v>78</v>
       </c>
-      <c r="B79" t="s">
-        <v>223</v>
-      </c>
-      <c r="C79">
-        <v>78181</v>
-      </c>
-      <c r="D79" t="s">
-        <v>223</v>
-      </c>
-      <c r="G79" t="str">
+      <c r="G79" t="e">
         <f t="shared" si="2"/>
-        <v>78 LinkSkillsToInternalInterview</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>